<commit_message>
additional mermaid integration with DMCAR excel format
</commit_message>
<xml_diff>
--- a/IDE/payment_example.xlsx
+++ b/IDE/payment_example.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="83">
   <si>
     <t xml:space="preserve">Namespace</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t xml:space="preserve">references the channel that handled the originating media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SomethingBad</t>
   </si>
   <si>
     <t xml:space="preserve">Mapping</t>
@@ -540,13 +543,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM8"/>
+  <dimension ref="A1:AM9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AL6" activeCellId="0" sqref="AL6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R10" activeCellId="0" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
@@ -891,6 +894,11 @@
         <v>52</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R9" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -913,7 +921,7 @@
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="4" style="0" width="22.36"/>
   </cols>
@@ -926,34 +934,34 @@
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -978,7 +986,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
@@ -991,22 +999,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>